<commit_message>
New Api added into 'settlement'
</commit_message>
<xml_diff>
--- a/zero-fm/src/main/resources/plugin/fm/oob/cab/fm.bill.process.xlsx
+++ b/zero-fm/src/main/resources/plugin/fm/oob/cab/fm.bill.process.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-fm/src/main/resources/plugin/fm/oob/cab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/web-app/workshop/zero-ws/zero-extension/zero-fm/src/main/resources/plugin/fm/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5D0461-C28E-C84F-A0EC-D7CC03F64BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C47539F-A3B8-F74A-A85E-23AA65279F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41720" yWindow="-9380" windowWidth="43000" windowHeight="26980" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="-68600" yWindow="-4520" windowWidth="43000" windowHeight="26980" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="190">
   <si>
     <t>key</t>
   </si>
@@ -684,6 +684,30 @@
   <si>
     <t>/api/bills/search/full</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标准结算</t>
+  </si>
+  <si>
+    <t>res.settle.finish</t>
+  </si>
+  <si>
+    <t>fm.settlement</t>
+  </si>
+  <si>
+    <t>2e8f3dc9-31de-4112-b330-92e27f6f34ac</t>
+  </si>
+  <si>
+    <t>8ddf8071-a15c-4069-801d-35eaa968c992</t>
+  </si>
+  <si>
+    <t>act.settle.finish</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>/api/settle/finish/:key</t>
   </si>
 </sst>
 </file>
@@ -694,34 +718,34 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FF0070C0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -729,7 +753,7 @@
     <font>
       <sz val="16"/>
       <color rgb="FF0070C0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -750,7 +774,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -902,20 +926,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -924,7 +944,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1333,1343 +1353,1395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="54.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="54.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11" style="3"/>
+    <col min="1" max="1" width="54.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="54.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" s="25" customFormat="1">
-      <c r="A2" s="22" t="s">
+    </row>
+    <row r="2" spans="1:9" s="23" customFormat="1">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-    </row>
-    <row r="3" spans="1:9" s="25" customFormat="1">
-      <c r="A3" s="26" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" s="23" customFormat="1">
+      <c r="A3" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="25" customFormat="1">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:9" s="23" customFormat="1">
+      <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="25" customFormat="1">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:9" s="23" customFormat="1">
+      <c r="A5" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="25" customFormat="1">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:9" s="23" customFormat="1">
+      <c r="A6" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="25" customFormat="1">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:9" s="23" customFormat="1">
+      <c r="A7" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="25" customFormat="1">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:9" s="23" customFormat="1">
+      <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="25" customFormat="1">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:9" s="23" customFormat="1">
+      <c r="A9" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="26" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="6"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="9"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="15" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="15" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="H25" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="I25" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="19" t="str">
-        <f t="shared" ref="B26:B28" si="0">A48</f>
+      <c r="B26" s="17" t="str">
+        <f t="shared" ref="B26:B28" si="0">A49</f>
         <v>3b6d1dc1-1266-4a26-abca-491fc804d1df</v>
       </c>
-      <c r="C26" s="19" t="str">
+      <c r="C26" s="17" t="str">
         <f>A$15</f>
         <v>2218a442-193e-4a66-8e27-89010e596720</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="15">
         <v>1</v>
       </c>
-      <c r="I26" s="17"/>
+      <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="19" t="str">
+      <c r="B27" s="17" t="str">
         <f t="shared" si="0"/>
         <v>543c5fad-ad2a-4912-85b0-8f7a75bd2887</v>
       </c>
-      <c r="C27" s="19" t="str">
+      <c r="C27" s="17" t="str">
         <f t="shared" ref="C27:C28" si="1">A$15</f>
         <v>2218a442-193e-4a66-8e27-89010e596720</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="H27" s="17">
+      <c r="H27" s="15">
         <v>1</v>
       </c>
-      <c r="I27" s="17"/>
+      <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="B28" s="19" t="str">
+      <c r="B28" s="17" t="str">
         <f t="shared" si="0"/>
         <v>c2d46a6e-9009-4990-a7e3-813c5a6ba634</v>
       </c>
-      <c r="C28" s="19" t="str">
+      <c r="C28" s="17" t="str">
         <f t="shared" si="1"/>
         <v>2218a442-193e-4a66-8e27-89010e596720</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="H28" s="17">
+      <c r="H28" s="15">
         <v>1</v>
       </c>
-      <c r="I28" s="17"/>
+      <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="19" t="str">
-        <f t="shared" ref="B29" si="2">A51</f>
+      <c r="B29" s="17" t="str">
+        <f t="shared" ref="B29" si="2">A52</f>
         <v>e3ba91f2-ca12-49a1-b911-f684eb21115d</v>
       </c>
-      <c r="C29" s="19" t="str">
+      <c r="C29" s="17" t="str">
         <f>A$16</f>
         <v>033886e3-9873-4602-b821-835d4c82792b</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F29" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G29" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H29" s="17">
+      <c r="H29" s="15">
         <v>4</v>
       </c>
-      <c r="I29" s="17"/>
+      <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="19" t="str">
-        <f t="shared" ref="B30:B36" si="3">A52</f>
+      <c r="B30" s="17" t="str">
+        <f t="shared" ref="B30:B37" si="3">A53</f>
         <v>5cd5e851-7596-4389-85fd-32fa11b4f6e6</v>
       </c>
-      <c r="C30" s="19" t="str">
+      <c r="C30" s="17" t="str">
         <f t="shared" ref="C30:C31" si="4">A$16</f>
         <v>033886e3-9873-4602-b821-835d4c82792b</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="17">
+      <c r="H30" s="15">
         <v>4</v>
       </c>
-      <c r="I30" s="17"/>
+      <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="19" t="str">
+      <c r="B31" s="17" t="str">
         <f t="shared" si="3"/>
         <v>e7f933c8-8584-4f34-a90f-1ebef8ca2e63</v>
       </c>
-      <c r="C31" s="19" t="str">
+      <c r="C31" s="17" t="str">
         <f t="shared" si="4"/>
         <v>033886e3-9873-4602-b821-835d4c82792b</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="H31" s="17">
+      <c r="H31" s="15">
         <v>4</v>
       </c>
-      <c r="I31" s="17"/>
+      <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="19" t="str">
+      <c r="B32" s="17" t="str">
         <f t="shared" si="3"/>
         <v>cdd4e0e5-90c8-4df1-8d3f-bdb8b28f25bd</v>
       </c>
-      <c r="C32" s="19" t="str">
+      <c r="C32" s="17" t="str">
         <f t="shared" ref="C32" si="5">A$16</f>
         <v>033886e3-9873-4602-b821-835d4c82792b</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="18" t="s">
+      <c r="F32" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="H32" s="17">
+      <c r="H32" s="15">
         <v>8</v>
       </c>
-      <c r="I32" s="17"/>
+      <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="19" t="str">
+      <c r="B33" s="17" t="str">
         <f t="shared" si="3"/>
         <v>2582df50-cae7-4bb9-a020-92d916dfeadb</v>
       </c>
-      <c r="C33" s="19" t="str">
+      <c r="C33" s="17" t="str">
         <f t="shared" ref="C33" si="6">A$16</f>
         <v>033886e3-9873-4602-b821-835d4c82792b</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="H33" s="17">
+      <c r="H33" s="15">
         <v>8</v>
       </c>
-      <c r="I33" s="17"/>
+      <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="19" t="str">
+      <c r="B34" s="17" t="str">
         <f t="shared" si="3"/>
         <v>4a652ed2-8f6f-4c5c-ac02-251135df04b3</v>
       </c>
-      <c r="C34" s="19" t="str">
+      <c r="C34" s="17" t="str">
         <f t="shared" ref="C34" si="7">A$16</f>
         <v>033886e3-9873-4602-b821-835d4c82792b</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="G34" s="17" t="s">
+      <c r="G34" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H34" s="15">
         <v>8</v>
       </c>
-      <c r="I34" s="17"/>
+      <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="19" t="str">
+      <c r="B35" s="17" t="str">
         <f t="shared" si="3"/>
         <v>f8ce2a9e-669c-4781-a125-a695217079c5</v>
       </c>
-      <c r="C35" s="19" t="str">
+      <c r="C35" s="17" t="str">
         <f t="shared" ref="C35" si="8">A$16</f>
         <v>033886e3-9873-4602-b821-835d4c82792b</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F35" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="G35" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="H35" s="17">
+      <c r="H35" s="15">
         <v>8</v>
       </c>
-      <c r="I35" s="17"/>
+      <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="19" t="str">
+      <c r="B36" s="17" t="str">
         <f t="shared" si="3"/>
         <v>9eef78da-a059-4998-8599-6f55c65091f7</v>
       </c>
-      <c r="C36" s="19" t="str">
+      <c r="C36" s="17" t="str">
         <f>A$17</f>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G36" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="H36" s="17">
+      <c r="H36" s="15">
         <v>4</v>
       </c>
-      <c r="I36" s="17"/>
+      <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" s="19" t="str">
-        <f t="shared" ref="B37" si="9">A59</f>
-        <v>2acce272-3eea-42e6-b468-2f11549555ff</v>
-      </c>
-      <c r="C37" s="19" t="str">
+      <c r="A37" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>2e8f3dc9-31de-4112-b330-92e27f6f34ac</v>
+      </c>
+      <c r="C37" s="17" t="str">
         <f>A$17</f>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
-      <c r="D37" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="H37" s="17">
-        <v>1</v>
-      </c>
-      <c r="I37" s="17"/>
+      <c r="D37" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="H37" s="15">
+        <v>8</v>
+      </c>
+      <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B38" s="19" t="str">
-        <f t="shared" ref="B38" si="10">A60</f>
-        <v>d0a2f099-5129-4f73-9a51-2154fd7ca0ef</v>
-      </c>
-      <c r="C38" s="19" t="str">
+      <c r="A38" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="17" t="str">
+        <f t="shared" ref="B38" si="9">A61</f>
+        <v>2acce272-3eea-42e6-b468-2f11549555ff</v>
+      </c>
+      <c r="C38" s="17" t="str">
         <f>A$17</f>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="H38" s="17">
-        <v>8</v>
-      </c>
-      <c r="I38" s="17"/>
+      <c r="D38" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H38" s="15">
+        <v>1</v>
+      </c>
+      <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B39" s="19" t="str">
-        <f t="shared" ref="B39" si="11">A61</f>
-        <v>0ef5b968-2b3b-47c1-a810-617b5ab10122</v>
-      </c>
-      <c r="C39" s="19" t="str">
+      <c r="A39" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="17" t="str">
+        <f t="shared" ref="B39" si="10">A62</f>
+        <v>d0a2f099-5129-4f73-9a51-2154fd7ca0ef</v>
+      </c>
+      <c r="C39" s="17" t="str">
         <f>A$17</f>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39" s="15">
+        <v>8</v>
+      </c>
+      <c r="I39" s="15"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="17" t="str">
+        <f t="shared" ref="B40" si="11">A63</f>
+        <v>0ef5b968-2b3b-47c1-a810-617b5ab10122</v>
+      </c>
+      <c r="C40" s="17" t="str">
+        <f>A$17</f>
+        <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
+      </c>
+      <c r="D40" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E40" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="F40" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="G39" s="17" t="s">
+      <c r="G40" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="H39" s="17">
+      <c r="H40" s="15">
         <v>8</v>
       </c>
-      <c r="I39" s="17"/>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="15" t="s">
+      <c r="I40" s="15"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="19" t="str">
-        <f>A62</f>
+      <c r="B41" s="17" t="str">
+        <f>A64</f>
         <v>d7aa419b-737e-4d21-8b0f-4adbd95820ee</v>
       </c>
-      <c r="C40" s="19" t="str">
+      <c r="C41" s="17" t="str">
         <f>A$19</f>
         <v>51541af0-7541-4abb-8208-0425ecc1dee8</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D41" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E41" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F41" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G41" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="H40" s="17">
+      <c r="H41" s="15">
         <v>4</v>
       </c>
-      <c r="I40" s="17"/>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="15" t="s">
+      <c r="I41" s="15"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="B41" s="19" t="str">
-        <f t="shared" ref="B41" si="12">A63</f>
+      <c r="B42" s="17" t="str">
+        <f t="shared" ref="B42" si="12">A65</f>
         <v>bbb0a9b5-bb93-4d52-824e-e3082a35b48d</v>
       </c>
-      <c r="C41" s="19" t="str">
+      <c r="C42" s="17" t="str">
         <f>A$19</f>
         <v>51541af0-7541-4abb-8208-0425ecc1dee8</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D42" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E42" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F42" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="G41" s="17" t="s">
+      <c r="G42" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="H41" s="17">
+      <c r="H42" s="15">
         <v>12</v>
       </c>
-      <c r="I41" s="17"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="3"/>
-      <c r="K42" s="4"/>
+      <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="3"/>
-      <c r="K43" s="4"/>
+      <c r="A43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="2"/>
+      <c r="K43" s="1"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="3"/>
-      <c r="K44" s="4"/>
+      <c r="A44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="2"/>
+      <c r="K44" s="1"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="2"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B46" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="30" t="s">
+      <c r="C46" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="10" t="s">
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B47" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C47" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D47" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E47" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F47" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="G47" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H47" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="I46" s="21" t="s">
+      <c r="I47" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="12" t="s">
+    <row r="48" spans="1:11">
+      <c r="A48" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B48" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C48" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D48" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E48" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F48" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G47" s="12" t="s">
+      <c r="G48" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H47" s="12" t="s">
+      <c r="H48" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I47" s="12" t="s">
+      <c r="I48" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="15" t="s">
+    <row r="49" spans="1:11">
+      <c r="A49" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B49" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C49" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D49" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E49" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F49" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G48" s="17">
+      <c r="G49" s="15">
         <v>1</v>
       </c>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="15" t="s">
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B50" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C50" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D50" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E50" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F50" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G49" s="17">
+      <c r="G50" s="15">
         <v>1</v>
       </c>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="15" t="s">
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B51" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C51" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D51" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="E51" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F51" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G50" s="17">
+      <c r="G51" s="15">
         <v>1</v>
       </c>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="15" t="s">
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B52" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C52" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D51" s="18" t="s">
+      <c r="D52" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="E52" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F52" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G51" s="17">
+      <c r="G52" s="15">
         <v>4</v>
       </c>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="15" t="s">
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B53" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C53" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D53" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E53" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F53" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G52" s="17">
+      <c r="G53" s="15">
         <v>4</v>
       </c>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="15" t="s">
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B54" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C54" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D54" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E54" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F54" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G53" s="17">
+      <c r="G54" s="15">
         <v>4</v>
       </c>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="15" t="s">
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B55" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C55" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="18" t="s">
+      <c r="D55" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E55" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F55" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G54" s="17">
+      <c r="G55" s="15">
         <v>8</v>
       </c>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="15" t="s">
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B56" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C56" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="D56" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E56" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F55" s="17" t="s">
+      <c r="F56" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G55" s="17">
+      <c r="G56" s="15">
         <v>8</v>
       </c>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="15" t="s">
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B57" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C57" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="D57" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E57" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F57" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G56" s="17">
+      <c r="G57" s="15">
         <v>8</v>
       </c>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="15" t="s">
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B58" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C58" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="18" t="s">
+      <c r="D58" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E58" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F57" s="17" t="s">
+      <c r="F58" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G57" s="17">
+      <c r="G58" s="15">
         <v>8</v>
       </c>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="15" t="s">
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B59" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C59" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D59" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="E58" s="17" t="s">
+      <c r="E59" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="F58" s="17" t="s">
+      <c r="F59" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G58" s="17">
+      <c r="G59" s="15">
         <v>4</v>
       </c>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" s="15" t="s">
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G60" s="15">
+        <v>8</v>
+      </c>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B61" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C61" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="18" t="s">
+      <c r="D61" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E61" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F59" s="17" t="s">
+      <c r="F61" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G59" s="17">
+      <c r="G61" s="15">
         <v>1</v>
       </c>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" s="15" t="s">
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B62" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C62" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D60" s="18" t="s">
+      <c r="D62" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E62" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="F60" s="17" t="s">
+      <c r="F62" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G60" s="17">
+      <c r="G62" s="15">
         <v>8</v>
       </c>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
-      <c r="K60" s="4"/>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="15" t="s">
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B63" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C63" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D63" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="E63" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F61" s="17" t="s">
+      <c r="F63" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G61" s="17">
+      <c r="G63" s="15">
         <v>8</v>
       </c>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="K61" s="4"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="15" t="s">
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B64" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="C64" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D64" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E64" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="F62" s="17" t="s">
+      <c r="F64" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G62" s="17">
+      <c r="G64" s="15">
         <v>4</v>
       </c>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="15" t="s">
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B65" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C65" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D65" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="E65" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="F63" s="17" t="s">
+      <c r="F65" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G63" s="17">
+      <c r="G65" s="15">
         <v>12</v>
       </c>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C46:I46"/>
     <mergeCell ref="C23:I23"/>
     <mergeCell ref="C2:D2"/>
   </mergeCells>

</xml_diff>

<commit_message>
API of new FM
</commit_message>
<xml_diff>
--- a/zero-fm/src/main/resources/plugin/fm/oob/cab/fm.bill.process.xlsx
+++ b/zero-fm/src/main/resources/plugin/fm/oob/cab/fm.bill.process.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/web-app/workshop/zero-ws/zero-extension/zero-fm/src/main/resources/plugin/fm/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEC9C3B-AA88-9743-A5A3-11D382D59A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DC8ED4-A74A-304F-A5CC-DC03F2DF018C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68600" yWindow="-4520" windowWidth="43000" windowHeight="26980" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="0" yWindow="1240" windowWidth="59840" windowHeight="36200" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="210">
   <si>
     <t>key</t>
   </si>
@@ -716,6 +716,54 @@
   </si>
   <si>
     <t>ab324585-f6ed-49bd-a7de-adbc21963ddf</t>
+  </si>
+  <si>
+    <t>cfec8dd9-8109-4a81-9685-1eb54608b5f1</t>
+  </si>
+  <si>
+    <t>71fd770a-8039-4a9b-95dc-fa5144c19796</t>
+  </si>
+  <si>
+    <t>res.settle.batch.qr</t>
+  </si>
+  <si>
+    <t>fm.settlement</t>
+  </si>
+  <si>
+    <t>fm.debt</t>
+  </si>
+  <si>
+    <t>resource.fm</t>
+  </si>
+  <si>
+    <t>83f85204-3f26-4ab6-bde5-7cee6074a909</t>
+  </si>
+  <si>
+    <t>4895b080-3684-4136-84cc-7b1a7db600c8</t>
+  </si>
+  <si>
+    <t>act.settle.batch.qr</t>
+  </si>
+  <si>
+    <t>res.debt.batch.qr</t>
+  </si>
+  <si>
+    <t>act.debt.batch.qr</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/api/settlement/batch</t>
+  </si>
+  <si>
+    <t>批读结算单</t>
+  </si>
+  <si>
+    <t>批读应收/应退</t>
+  </si>
+  <si>
+    <t>/api/debt/batch</t>
   </si>
 </sst>
 </file>
@@ -1361,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
@@ -1729,7 +1777,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="17" t="str">
-        <f t="shared" ref="B26:B28" si="0">A50</f>
+        <f t="shared" ref="B26:B28" si="0">A52</f>
         <v>3b6d1dc1-1266-4a26-abca-491fc804d1df</v>
       </c>
       <c r="C26" s="17" t="str">
@@ -1816,7 +1864,7 @@
         <v>62</v>
       </c>
       <c r="B29" s="17" t="str">
-        <f t="shared" ref="B29" si="2">A53</f>
+        <f t="shared" ref="B29" si="2">A55</f>
         <v>e3ba91f2-ca12-49a1-b911-f684eb21115d</v>
       </c>
       <c r="C29" s="17" t="str">
@@ -1845,7 +1893,7 @@
         <v>67</v>
       </c>
       <c r="B30" s="17" t="str">
-        <f t="shared" ref="B30:B38" si="3">A54</f>
+        <f t="shared" ref="B30:B37" si="3">A56</f>
         <v>5cd5e851-7596-4389-85fd-32fa11b4f6e6</v>
       </c>
       <c r="C30" s="17" t="str">
@@ -2023,7 +2071,7 @@
         <v>9eef78da-a059-4998-8599-6f55c65091f7</v>
       </c>
       <c r="C36" s="17" t="str">
-        <f>A$17</f>
+        <f t="shared" ref="C36:C41" si="9">A$17</f>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
       <c r="D36" s="16" t="s">
@@ -2052,7 +2100,7 @@
         <v>2e8f3dc9-31de-4112-b330-92e27f6f34ac</v>
       </c>
       <c r="C37" s="17" t="str">
-        <f>A$17</f>
+        <f t="shared" si="9"/>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
       <c r="D37" s="16" t="s">
@@ -2077,11 +2125,11 @@
         <v>193</v>
       </c>
       <c r="B38" s="17" t="str">
-        <f>A62</f>
+        <f>A64</f>
         <v>169b51c8-55e6-4167-8e49-963cebe155af</v>
       </c>
       <c r="C38" s="17" t="str">
-        <f>A$17</f>
+        <f t="shared" si="9"/>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
       <c r="D38" s="16" t="s">
@@ -2106,11 +2154,11 @@
         <v>131</v>
       </c>
       <c r="B39" s="17" t="str">
-        <f t="shared" ref="B39" si="9">A63</f>
+        <f t="shared" ref="B39" si="10">A65</f>
         <v>2acce272-3eea-42e6-b468-2f11549555ff</v>
       </c>
       <c r="C39" s="17" t="str">
-        <f>A$17</f>
+        <f t="shared" si="9"/>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
       <c r="D39" s="16" t="s">
@@ -2135,11 +2183,11 @@
         <v>139</v>
       </c>
       <c r="B40" s="17" t="str">
-        <f t="shared" ref="B40" si="10">A64</f>
+        <f t="shared" ref="B40" si="11">A66</f>
         <v>d0a2f099-5129-4f73-9a51-2154fd7ca0ef</v>
       </c>
       <c r="C40" s="17" t="str">
-        <f>A$17</f>
+        <f t="shared" si="9"/>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
       <c r="D40" s="16" t="s">
@@ -2164,11 +2212,11 @@
         <v>145</v>
       </c>
       <c r="B41" s="17" t="str">
-        <f t="shared" ref="B41" si="11">A65</f>
+        <f t="shared" ref="B41:B43" si="12">A67</f>
         <v>0ef5b968-2b3b-47c1-a810-617b5ab10122</v>
       </c>
       <c r="C41" s="17" t="str">
-        <f>A$17</f>
+        <f t="shared" si="9"/>
         <v>40f9ae68-f5f2-4414-b424-a0345a62f1ea</v>
       </c>
       <c r="D41" s="16" t="s">
@@ -2190,79 +2238,119 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>cfec8dd9-8109-4a81-9685-1eb54608b5f1</v>
+      </c>
+      <c r="C42" s="17" t="str">
+        <f>A$15</f>
+        <v>2218a442-193e-4a66-8e27-89010e596720</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="H42" s="15">
+        <v>1</v>
+      </c>
+      <c r="I42" s="15"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>71fd770a-8039-4a9b-95dc-fa5144c19796</v>
+      </c>
+      <c r="C43" s="17" t="str">
+        <f>A$15</f>
+        <v>2218a442-193e-4a66-8e27-89010e596720</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="H43" s="15">
+        <v>1</v>
+      </c>
+      <c r="I43" s="15"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B42" s="17" t="str">
-        <f>A66</f>
+      <c r="B44" s="17" t="str">
+        <f>A70</f>
         <v>d7aa419b-737e-4d21-8b0f-4adbd95820ee</v>
       </c>
-      <c r="C42" s="17" t="str">
+      <c r="C44" s="17" t="str">
         <f>A$19</f>
         <v>51541af0-7541-4abb-8208-0425ecc1dee8</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D44" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E44" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F44" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G44" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H44" s="15">
         <v>4</v>
       </c>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="13" t="s">
+      <c r="I44" s="15"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B43" s="17" t="str">
-        <f t="shared" ref="B43" si="12">A67</f>
+      <c r="B45" s="17" t="str">
+        <f t="shared" ref="B45" si="13">A71</f>
         <v>bbb0a9b5-bb93-4d52-824e-e3082a35b48d</v>
       </c>
-      <c r="C43" s="17" t="str">
+      <c r="C45" s="17" t="str">
         <f>A$19</f>
         <v>51541af0-7541-4abb-8208-0425ecc1dee8</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D45" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E45" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F45" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="G43" s="15" t="s">
+      <c r="G45" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H45" s="15">
         <v>12</v>
       </c>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="2"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="2"/>
-      <c r="K45" s="1"/>
+      <c r="I45" s="15"/>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1"/>
@@ -2274,142 +2362,110 @@
       <c r="K46" s="1"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="2"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="2"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B49" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C49" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="8" t="s">
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C50" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F50" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G48" s="19" t="s">
+      <c r="G50" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H48" s="19" t="s">
+      <c r="H50" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="I48" s="19" t="s">
+      <c r="I50" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="10" t="s">
+    <row r="51" spans="1:9">
+      <c r="A51" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B51" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D51" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E51" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F51" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G49" s="10" t="s">
+      <c r="G51" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="10" t="s">
+      <c r="H51" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I49" s="10" t="s">
+      <c r="I51" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="13" t="s">
+    <row r="52" spans="1:9">
+      <c r="A52" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B52" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G50" s="15">
-        <v>1</v>
-      </c>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G51" s="15">
-        <v>1</v>
-      </c>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>167</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>164</v>
+        <v>54</v>
       </c>
       <c r="E52" s="15" t="s">
         <v>47</v>
@@ -2423,18 +2479,18 @@
       <c r="H52" s="15"/>
       <c r="I52" s="15"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:9">
       <c r="A53" s="13" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>59</v>
+        <v>166</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>58</v>
+        <v>165</v>
       </c>
       <c r="E53" s="15" t="s">
         <v>47</v>
@@ -2443,23 +2499,23 @@
         <v>120</v>
       </c>
       <c r="G53" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:9">
       <c r="A54" s="13" t="s">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>66</v>
+        <v>167</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="E54" s="15" t="s">
         <v>47</v>
@@ -2468,23 +2524,23 @@
         <v>120</v>
       </c>
       <c r="G54" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H54" s="15"/>
       <c r="I54" s="15"/>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:9">
       <c r="A55" s="13" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E55" s="15" t="s">
         <v>47</v>
@@ -2498,18 +2554,18 @@
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:9">
       <c r="A56" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E56" s="15" t="s">
         <v>47</v>
@@ -2518,23 +2574,23 @@
         <v>120</v>
       </c>
       <c r="G56" s="15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H56" s="15"/>
       <c r="I56" s="15"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:9">
       <c r="A57" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E57" s="15" t="s">
         <v>47</v>
@@ -2543,23 +2599,23 @@
         <v>120</v>
       </c>
       <c r="G57" s="15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H57" s="15"/>
       <c r="I57" s="15"/>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:9">
       <c r="A58" s="13" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>47</v>
@@ -2573,18 +2629,18 @@
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:9">
       <c r="A59" s="13" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>47</v>
@@ -2598,68 +2654,68 @@
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:9">
       <c r="A60" s="13" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>185</v>
+        <v>88</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>190</v>
+        <v>86</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="F60" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G60" s="15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H60" s="15"/>
       <c r="I60" s="15"/>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:9">
       <c r="A61" s="13" t="s">
-        <v>178</v>
+        <v>96</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>186</v>
+        <v>95</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>191</v>
+        <v>94</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="F61" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G61" s="15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:9">
       <c r="A62" s="13" t="s">
-        <v>189</v>
+        <v>127</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E62" s="15" t="s">
         <v>101</v>
@@ -2673,69 +2729,68 @@
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:9">
       <c r="A63" s="13" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>126</v>
+        <v>191</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="F63" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G63" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H63" s="15"/>
       <c r="I63" s="15"/>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:9">
       <c r="A64" s="13" t="s">
-        <v>136</v>
+        <v>189</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="F64" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G64" s="15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
-      <c r="K64" s="1"/>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="13" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E65" s="15" t="s">
         <v>123</v>
@@ -2744,66 +2799,169 @@
         <v>120</v>
       </c>
       <c r="G65" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H65" s="15"/>
       <c r="I65" s="15"/>
-      <c r="K65" s="1"/>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="13" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="F66" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G66" s="15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H66" s="15"/>
       <c r="I66" s="15"/>
+      <c r="K66" s="1"/>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="13" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="F67" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G67" s="15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
+      <c r="K67" s="1"/>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="G68" s="15">
+        <v>1</v>
+      </c>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="K68" s="1"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="G69" s="15">
+        <v>1</v>
+      </c>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="K69" s="1"/>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G70" s="15">
+        <v>4</v>
+      </c>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D71" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G71" s="15">
+        <v>12</v>
+      </c>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C49:I49"/>
     <mergeCell ref="C23:I23"/>
     <mergeCell ref="C2:D2"/>
   </mergeCells>

</xml_diff>